<commit_message>
changes to dataschema: Immigration variable labelling now 0 = no, 1 = yes adjustments in DD and DPE for variable input of dkmd instead of admd (acc. to Mrs Schneider)
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2586E51B-EE1B-4AD7-8441-8D3F8A05EB38}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC8B4E2-1EBB-45C8-B8DA-215560BF0A03}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F66E816F-B844-4025-9D57-703EE86FBE35}"/>
   </bookViews>
@@ -295,9 +295,6 @@
     <t>polyunsaturated fat</t>
   </si>
   <si>
-    <t>admd</t>
-  </si>
-  <si>
     <t>total sugar</t>
   </si>
   <si>
@@ -785,6 +782,9 @@
   </si>
   <si>
     <t>all kinds of minced meat</t>
+  </si>
+  <si>
+    <t>dkmd</t>
   </si>
 </sst>
 </file>
@@ -1333,8 +1333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2CBB1F-BD60-4F64-AB96-FAE7D77C8064}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -1423,7 +1423,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C6" s="16" t="s">
         <v>12</v>
@@ -1647,10 +1647,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>242</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>243</v>
       </c>
       <c r="D22" s="18" t="s">
         <v>7</v>
@@ -1661,7 +1661,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C23" s="16" t="s">
         <v>44</v>
@@ -1675,7 +1675,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C24" s="16" t="s">
         <v>45</v>
@@ -1689,7 +1689,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C25" s="16" t="s">
         <v>46</v>
@@ -1773,7 +1773,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>57</v>
@@ -1787,7 +1787,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C32" s="32" t="s">
         <v>58</v>
@@ -2011,10 +2011,10 @@
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>89</v>
-      </c>
-      <c r="C48" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>17</v>
@@ -2025,10 +2025,10 @@
         <v>48</v>
       </c>
       <c r="B49" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="6" t="s">
         <v>91</v>
-      </c>
-      <c r="C49" s="6" t="s">
-        <v>92</v>
       </c>
       <c r="D49" s="3" t="s">
         <v>17</v>
@@ -2039,10 +2039,10 @@
         <v>49</v>
       </c>
       <c r="B50" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C50" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="C50" s="6" t="s">
-        <v>94</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>17</v>
@@ -2053,10 +2053,10 @@
         <v>50</v>
       </c>
       <c r="B51" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>17</v>
@@ -2067,10 +2067,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C52" s="18" t="s">
         <v>97</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>98</v>
       </c>
       <c r="D52" t="s">
         <v>17</v>
@@ -2081,10 +2081,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C53" s="25" t="s">
         <v>99</v>
-      </c>
-      <c r="C53" s="25" t="s">
-        <v>100</v>
       </c>
       <c r="D53" t="s">
         <v>17</v>
@@ -2095,10 +2095,10 @@
         <v>53</v>
       </c>
       <c r="B54" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" s="25" t="s">
         <v>101</v>
-      </c>
-      <c r="C54" s="25" t="s">
-        <v>102</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
@@ -2109,10 +2109,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="25" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="25" t="s">
         <v>103</v>
-      </c>
-      <c r="C55" s="25" t="s">
-        <v>104</v>
       </c>
       <c r="D55" t="s">
         <v>17</v>
@@ -2123,10 +2123,10 @@
         <v>55</v>
       </c>
       <c r="B56" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="25" t="s">
         <v>105</v>
-      </c>
-      <c r="C56" s="25" t="s">
-        <v>106</v>
       </c>
       <c r="D56" t="s">
         <v>17</v>
@@ -2137,10 +2137,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="C57" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="C57" s="25" t="s">
-        <v>108</v>
       </c>
       <c r="D57" t="s">
         <v>17</v>
@@ -2151,10 +2151,10 @@
         <v>57</v>
       </c>
       <c r="B58" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="C58" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="C58" s="25" t="s">
-        <v>110</v>
       </c>
       <c r="D58" t="s">
         <v>17</v>
@@ -2165,10 +2165,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="C59" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="D59" t="s">
         <v>17</v>
@@ -2179,10 +2179,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="C60" s="4" t="s">
         <v>113</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>114</v>
       </c>
       <c r="D60" t="s">
         <v>17</v>
@@ -2193,10 +2193,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="C61" s="25" t="s">
         <v>115</v>
-      </c>
-      <c r="C61" s="25" t="s">
-        <v>116</v>
       </c>
       <c r="D61" t="s">
         <v>17</v>
@@ -2207,10 +2207,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C62" s="25" t="s">
         <v>117</v>
-      </c>
-      <c r="C62" s="25" t="s">
-        <v>118</v>
       </c>
       <c r="D62" t="s">
         <v>17</v>
@@ -2221,10 +2221,10 @@
         <v>62</v>
       </c>
       <c r="B63" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="C63" s="25" t="s">
         <v>119</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>120</v>
       </c>
       <c r="D63" t="s">
         <v>17</v>
@@ -2235,10 +2235,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="25" t="s">
+        <v>120</v>
+      </c>
+      <c r="C64" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="C64" s="25" t="s">
-        <v>122</v>
       </c>
       <c r="D64" t="s">
         <v>17</v>
@@ -2249,10 +2249,10 @@
         <v>64</v>
       </c>
       <c r="B65" s="25" t="s">
+        <v>122</v>
+      </c>
+      <c r="C65" s="25" t="s">
         <v>123</v>
-      </c>
-      <c r="C65" s="25" t="s">
-        <v>124</v>
       </c>
       <c r="D65" t="s">
         <v>17</v>
@@ -2263,10 +2263,10 @@
         <v>65</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C66" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>126</v>
       </c>
       <c r="D66" t="s">
         <v>17</v>
@@ -2277,10 +2277,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C67" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>128</v>
       </c>
       <c r="D67" t="s">
         <v>17</v>
@@ -2291,10 +2291,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C68" s="4" t="s">
         <v>129</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>130</v>
       </c>
       <c r="D68" t="s">
         <v>17</v>
@@ -2305,10 +2305,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>131</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>132</v>
       </c>
       <c r="D69" t="s">
         <v>17</v>
@@ -2319,10 +2319,10 @@
         <v>69</v>
       </c>
       <c r="B70" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C70" s="4" t="s">
         <v>133</v>
-      </c>
-      <c r="C70" s="4" t="s">
-        <v>134</v>
       </c>
       <c r="D70" t="s">
         <v>17</v>
@@ -2333,10 +2333,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C71" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>136</v>
       </c>
       <c r="D71" t="s">
         <v>17</v>
@@ -2347,10 +2347,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C72" s="25" t="s">
         <v>137</v>
-      </c>
-      <c r="C72" s="25" t="s">
-        <v>138</v>
       </c>
       <c r="D72" t="s">
         <v>17</v>
@@ -2361,10 +2361,10 @@
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="8" t="s">
         <v>139</v>
-      </c>
-      <c r="C73" s="8" t="s">
-        <v>140</v>
       </c>
       <c r="D73" t="s">
         <v>17</v>
@@ -2375,10 +2375,10 @@
         <v>73</v>
       </c>
       <c r="B74" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="C74" s="24" t="s">
         <v>141</v>
-      </c>
-      <c r="C74" s="24" t="s">
-        <v>142</v>
       </c>
       <c r="D74" t="s">
         <v>17</v>
@@ -2389,10 +2389,10 @@
         <v>74</v>
       </c>
       <c r="B75" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="C75" s="25" t="s">
         <v>143</v>
-      </c>
-      <c r="C75" s="25" t="s">
-        <v>144</v>
       </c>
       <c r="D75" t="s">
         <v>17</v>
@@ -2403,10 +2403,10 @@
         <v>75</v>
       </c>
       <c r="B76" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="C76" s="25" t="s">
         <v>145</v>
-      </c>
-      <c r="C76" s="25" t="s">
-        <v>146</v>
       </c>
       <c r="D76" t="s">
         <v>17</v>
@@ -2417,10 +2417,10 @@
         <v>76</v>
       </c>
       <c r="B77" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="C77" s="25" t="s">
         <v>147</v>
-      </c>
-      <c r="C77" s="25" t="s">
-        <v>148</v>
       </c>
       <c r="D77" t="s">
         <v>17</v>
@@ -2431,10 +2431,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="26" t="s">
+        <v>148</v>
+      </c>
+      <c r="C78" s="27" t="s">
         <v>149</v>
-      </c>
-      <c r="C78" s="27" t="s">
-        <v>150</v>
       </c>
       <c r="D78" t="s">
         <v>17</v>
@@ -2445,10 +2445,10 @@
         <v>78</v>
       </c>
       <c r="B79" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="C79" s="25" t="s">
         <v>151</v>
-      </c>
-      <c r="C79" s="25" t="s">
-        <v>152</v>
       </c>
       <c r="D79" t="s">
         <v>17</v>
@@ -2459,10 +2459,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C80" s="25" t="s">
         <v>153</v>
-      </c>
-      <c r="C80" s="25" t="s">
-        <v>154</v>
       </c>
       <c r="D80" t="s">
         <v>17</v>
@@ -2473,10 +2473,10 @@
         <v>80</v>
       </c>
       <c r="B81" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="C81" s="25" t="s">
         <v>155</v>
-      </c>
-      <c r="C81" s="25" t="s">
-        <v>156</v>
       </c>
       <c r="D81" t="s">
         <v>17</v>
@@ -2487,10 +2487,10 @@
         <v>81</v>
       </c>
       <c r="B82" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C82" s="25" t="s">
         <v>157</v>
-      </c>
-      <c r="C82" s="25" t="s">
-        <v>158</v>
       </c>
       <c r="D82" t="s">
         <v>17</v>
@@ -2501,10 +2501,10 @@
         <v>82</v>
       </c>
       <c r="B83" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C83" s="25" t="s">
         <v>159</v>
-      </c>
-      <c r="C83" s="25" t="s">
-        <v>160</v>
       </c>
       <c r="D83" t="s">
         <v>17</v>
@@ -2515,10 +2515,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C84" s="8" t="s">
         <v>161</v>
-      </c>
-      <c r="C84" s="8" t="s">
-        <v>162</v>
       </c>
       <c r="D84" t="s">
         <v>17</v>
@@ -2529,10 +2529,10 @@
         <v>84</v>
       </c>
       <c r="B85" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="C85" s="24" t="s">
         <v>163</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>164</v>
       </c>
       <c r="D85" t="s">
         <v>17</v>
@@ -2543,10 +2543,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" s="8" t="s">
         <v>165</v>
-      </c>
-      <c r="C86" s="8" t="s">
-        <v>166</v>
       </c>
       <c r="D86" t="s">
         <v>17</v>
@@ -2557,10 +2557,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="C87" s="25" t="s">
         <v>167</v>
-      </c>
-      <c r="C87" s="25" t="s">
-        <v>168</v>
       </c>
       <c r="D87" t="s">
         <v>17</v>
@@ -2571,10 +2571,10 @@
         <v>87</v>
       </c>
       <c r="B88" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="C88" s="25" t="s">
         <v>169</v>
-      </c>
-      <c r="C88" s="25" t="s">
-        <v>170</v>
       </c>
       <c r="D88" t="s">
         <v>17</v>
@@ -2585,10 +2585,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C89" s="8" t="s">
         <v>171</v>
-      </c>
-      <c r="C89" s="8" t="s">
-        <v>172</v>
       </c>
       <c r="D89" t="s">
         <v>17</v>
@@ -2599,10 +2599,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="C90" s="25" t="s">
         <v>173</v>
-      </c>
-      <c r="C90" s="25" t="s">
-        <v>174</v>
       </c>
       <c r="D90" t="s">
         <v>17</v>
@@ -2613,10 +2613,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="C91" s="25" t="s">
         <v>175</v>
-      </c>
-      <c r="C91" s="25" t="s">
-        <v>176</v>
       </c>
       <c r="D91" t="s">
         <v>17</v>
@@ -2627,10 +2627,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="C92" s="25" t="s">
         <v>177</v>
-      </c>
-      <c r="C92" s="25" t="s">
-        <v>178</v>
       </c>
       <c r="D92" t="s">
         <v>17</v>
@@ -2641,10 +2641,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>179</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>180</v>
       </c>
       <c r="D93" t="s">
         <v>17</v>
@@ -2655,10 +2655,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" s="8" t="s">
         <v>181</v>
-      </c>
-      <c r="C94" s="8" t="s">
-        <v>182</v>
       </c>
       <c r="D94" t="s">
         <v>17</v>
@@ -2669,10 +2669,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="25" t="s">
+        <v>182</v>
+      </c>
+      <c r="C95" s="25" t="s">
         <v>183</v>
-      </c>
-      <c r="C95" s="25" t="s">
-        <v>184</v>
       </c>
       <c r="D95" t="s">
         <v>17</v>
@@ -2683,10 +2683,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="25" t="s">
+        <v>184</v>
+      </c>
+      <c r="C96" s="25" t="s">
         <v>185</v>
-      </c>
-      <c r="C96" s="25" t="s">
-        <v>186</v>
       </c>
       <c r="D96" t="s">
         <v>17</v>
@@ -2697,10 +2697,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="C97" s="25" t="s">
         <v>187</v>
-      </c>
-      <c r="C97" s="25" t="s">
-        <v>188</v>
       </c>
       <c r="D97" t="s">
         <v>17</v>
@@ -2711,10 +2711,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="C98" s="25" t="s">
         <v>189</v>
-      </c>
-      <c r="C98" s="25" t="s">
-        <v>190</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -2725,10 +2725,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="25" t="s">
+        <v>190</v>
+      </c>
+      <c r="C99" s="25" t="s">
         <v>191</v>
-      </c>
-      <c r="C99" s="25" t="s">
-        <v>192</v>
       </c>
       <c r="D99" t="s">
         <v>17</v>
@@ -2739,10 +2739,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="C100" s="25" t="s">
         <v>193</v>
-      </c>
-      <c r="C100" s="25" t="s">
-        <v>194</v>
       </c>
       <c r="D100" t="s">
         <v>17</v>
@@ -2753,10 +2753,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="25" t="s">
+        <v>194</v>
+      </c>
+      <c r="C101" s="25" t="s">
         <v>195</v>
-      </c>
-      <c r="C101" s="25" t="s">
-        <v>196</v>
       </c>
       <c r="D101" t="s">
         <v>17</v>
@@ -2767,10 +2767,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="C102" s="25" t="s">
         <v>197</v>
-      </c>
-      <c r="C102" s="25" t="s">
-        <v>198</v>
       </c>
       <c r="D102" t="s">
         <v>17</v>
@@ -2781,10 +2781,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C103" s="8" t="s">
         <v>199</v>
-      </c>
-      <c r="C103" s="8" t="s">
-        <v>200</v>
       </c>
       <c r="D103" t="s">
         <v>17</v>
@@ -2795,10 +2795,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="8" t="s">
         <v>201</v>
-      </c>
-      <c r="C104" s="8" t="s">
-        <v>202</v>
       </c>
       <c r="D104" t="s">
         <v>17</v>
@@ -2809,10 +2809,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="C105" s="8" t="s">
         <v>203</v>
-      </c>
-      <c r="C105" s="8" t="s">
-        <v>204</v>
       </c>
       <c r="D105" t="s">
         <v>17</v>
@@ -2823,10 +2823,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C106" s="8" t="s">
         <v>205</v>
-      </c>
-      <c r="C106" s="8" t="s">
-        <v>206</v>
       </c>
       <c r="D106" t="s">
         <v>17</v>
@@ -2837,10 +2837,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>207</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>208</v>
       </c>
       <c r="D107" t="s">
         <v>17</v>
@@ -2851,10 +2851,10 @@
         <v>107</v>
       </c>
       <c r="B108" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="C108" s="25" t="s">
         <v>209</v>
-      </c>
-      <c r="C108" s="25" t="s">
-        <v>210</v>
       </c>
       <c r="D108" t="s">
         <v>17</v>
@@ -2865,10 +2865,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="C109" s="25" t="s">
         <v>211</v>
-      </c>
-      <c r="C109" s="25" t="s">
-        <v>212</v>
       </c>
       <c r="D109" t="s">
         <v>17</v>
@@ -2879,10 +2879,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="C110" s="25" t="s">
         <v>213</v>
-      </c>
-      <c r="C110" s="25" t="s">
-        <v>214</v>
       </c>
       <c r="D110" t="s">
         <v>17</v>
@@ -2893,10 +2893,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C111" s="25" t="s">
         <v>215</v>
-      </c>
-      <c r="C111" s="25" t="s">
-        <v>216</v>
       </c>
       <c r="D111" t="s">
         <v>17</v>
@@ -2907,10 +2907,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C112" s="25" t="s">
         <v>217</v>
-      </c>
-      <c r="C112" s="25" t="s">
-        <v>218</v>
       </c>
       <c r="D112" t="s">
         <v>17</v>
@@ -2921,10 +2921,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C113" s="18" t="s">
         <v>251</v>
-      </c>
-      <c r="C113" s="18" t="s">
-        <v>252</v>
       </c>
       <c r="D113" t="s">
         <v>17</v>
@@ -2953,7 +2953,7 @@
   <sheetData>
     <row r="1" spans="1:4" s="22" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>1</v>
@@ -2962,7 +2962,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2973,7 +2973,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2984,7 +2984,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2995,7 +2995,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3017,7 +3017,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3028,7 +3028,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3050,84 +3050,84 @@
         <v>5</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B10" s="33">
         <v>1</v>
       </c>
       <c r="C10" s="33" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B11" s="33">
         <v>2</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B12" s="33">
         <v>3</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B13" s="33">
         <v>4</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B14" s="33">
         <v>5</v>
       </c>
       <c r="C14" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B15" s="33">
         <v>6</v>
       </c>
       <c r="C15" s="16" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B16" s="33">
         <v>7</v>
       </c>
       <c r="C16" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -3138,7 +3138,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -3149,7 +3149,7 @@
         <v>2</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -3160,7 +3160,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -3171,7 +3171,7 @@
         <v>4</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -3182,7 +3182,7 @@
         <v>0</v>
       </c>
       <c r="C21" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -3193,7 +3193,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -3204,7 +3204,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -3215,29 +3215,29 @@
         <v>1</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B25" s="17">
         <v>0</v>
       </c>
       <c r="C25" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B26" s="17">
         <v>1</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3248,7 +3248,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -3259,7 +3259,7 @@
         <v>1</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -3270,7 +3270,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -3281,7 +3281,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>0</v>
       </c>
       <c r="C31" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -3303,7 +3303,7 @@
         <v>1</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="C33" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3325,7 +3325,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -3336,7 +3336,7 @@
         <v>0</v>
       </c>
       <c r="C35" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -3347,7 +3347,7 @@
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
@@ -3358,7 +3358,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -3369,7 +3369,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -3380,7 +3380,7 @@
         <v>0</v>
       </c>
       <c r="C39" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
@@ -3391,7 +3391,7 @@
         <v>1</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
@@ -3402,7 +3402,7 @@
         <v>0</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -3413,7 +3413,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -3424,7 +3424,7 @@
         <v>0</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -3435,7 +3435,7 @@
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
@@ -4380,6 +4380,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4620,15 +4629,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4642,6 +4642,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373398BC-AB18-4DB6-A1F8-8358A59BBA75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B7B5203-47B3-4C9D-894E-AFE841918B2A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4660,14 +4668,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373398BC-AB18-4DB6-A1F8-8358A59BBA75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84A691B-EF98-4CD8-ACB1-815521123DAC}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
adding categories (0/1) for 5 variables shown in S1_P2 but not S3_P2 as discussed via e-mail
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schwarz-f\Desktop\use-cases-harmonisation\rmonize\data_dictionary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9D0435-22F2-4D3B-9C42-B4C142482E22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B184D0F-96F9-4649-8F74-537C232596CA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" xr2:uid="{F66E816F-B844-4025-9D57-703EE86FBE35}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14028" activeTab="1" xr2:uid="{F66E816F-B844-4025-9D57-703EE86FBE35}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="253">
   <si>
     <t>index</t>
   </si>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2CBB1F-BD60-4F64-AB96-FAE7D77C8064}">
   <dimension ref="A1:F113"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E113" sqref="A1:E113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1385,493 +1385,495 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3">
-        <v>3</v>
+      <c r="A4">
+        <v>4</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>12</v>
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>14</v>
       </c>
       <c r="D5" s="18" t="s">
         <v>6</v>
       </c>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="18" t="s">
+      <c r="A6">
         <v>6</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="3">
+        <v>19</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>20</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="5" t="s">
+      <c r="A9" s="3">
         <v>21</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
+      <c r="B9" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10">
         <v>22</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="B10" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
         <v>23</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="30" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>24</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="B12" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
         <v>25</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14">
         <v>26</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
+      <c r="B14" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>30</v>
+      </c>
+      <c r="B16" s="31" t="s">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>31</v>
+      </c>
+      <c r="B17" s="31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
         <v>32</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="3">
-        <v>17</v>
-      </c>
       <c r="B18" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
+        <v>68</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" t="s">
-        <v>19</v>
+        <v>73</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D20" s="18" t="s">
+      <c r="A20">
+        <v>36</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="18" t="s">
+      <c r="A21" s="3">
+        <v>37</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
+        <v>3</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>7</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>8</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="C22" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23">
+      <c r="D24" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>9</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="3">
+      <c r="C25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D24" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25">
+      <c r="D25" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>10</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3">
+      <c r="C26" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A27">
+      <c r="D26" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>11</v>
+      </c>
+      <c r="B27" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>57</v>
+      <c r="C27" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A28" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>12</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>13</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>14</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>15</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>16</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>17</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
         <v>27</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B35" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C35" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="3">
-        <v>29</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="D30" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D31" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D32" s="18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3">
-        <v>33</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>6</v>
+      <c r="D35" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>36</v>
+      <c r="A37" s="3">
+        <v>33</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>6</v>
+        <v>70</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D37" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>6</v>
+        <v>74</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -2925,6 +2927,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:E113">
+    <sortCondition descending="1" ref="D2:D113"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2934,8 +2939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E2A9C4F-4DB8-4E79-A3FD-0B1BDC762B9F}">
   <dimension ref="A1:D347"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="O42" sqref="O42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3433,54 +3438,114 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="16"/>
+      <c r="A45" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B45" s="17">
+        <v>0</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="17"/>
-      <c r="C46" s="4"/>
+      <c r="A46" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="B46" s="17">
+        <v>1</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="17"/>
-      <c r="C47" s="16"/>
+      <c r="A47" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B47" s="17">
+        <v>0</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
-      <c r="B48" s="17"/>
-      <c r="C48" s="4"/>
+      <c r="A48" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="B48" s="17">
+        <v>1</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="17"/>
-      <c r="C49" s="16"/>
+      <c r="A49" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49" s="17">
+        <v>0</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-      <c r="B50" s="17"/>
-      <c r="C50" s="4"/>
+      <c r="A50" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="17">
+        <v>1</v>
+      </c>
+      <c r="C50" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="17"/>
-      <c r="C51" s="16"/>
+      <c r="A51" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="17">
+        <v>0</v>
+      </c>
+      <c r="C51" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="9"/>
-      <c r="B52" s="17"/>
-      <c r="C52" s="4"/>
+      <c r="A52" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="17">
+        <v>1</v>
+      </c>
+      <c r="C52" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="9"/>
-      <c r="B53" s="17"/>
-      <c r="C53" s="16"/>
+      <c r="A53" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53" s="17">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="9"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="4"/>
+      <c r="A54" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="17">
+        <v>1</v>
+      </c>
+      <c r="C54" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
@@ -4386,15 +4451,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4635,6 +4691,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84A691B-EF98-4CD8-ACB1-815521123DAC}">
   <ds:schemaRefs>
@@ -4653,14 +4718,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373398BC-AB18-4DB6-A1F8-8358A59BBA75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981C8453-1A31-4F97-BF69-09535CFA9398}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4677,4 +4734,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373398BC-AB18-4DB6-A1F8-8358A59BBA75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Had a look again in the mail from Mrs. schneider. So the sugar variables should be correct!
</commit_message>
<xml_diff>
--- a/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
+++ b/rmonize/data_dictionary/DD_KORA_S3_P2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14030" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14030"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -786,13 +786,13 @@
     <t>disaccharides</t>
   </si>
   <si>
-    <t>dmosa</t>
-  </si>
-  <si>
-    <t>ddisa</t>
-  </si>
-  <si>
     <t>I don't know</t>
+  </si>
+  <si>
+    <t>dkmosa</t>
+  </si>
+  <si>
+    <t>dkdisa</t>
   </si>
 </sst>
 </file>
@@ -1329,8 +1329,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2009,7 +2009,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>251</v>
@@ -2023,7 +2023,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>252</v>
@@ -2955,7 +2955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D349"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
@@ -3527,7 +3527,7 @@
         <v>2</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -3560,7 +3560,7 @@
         <v>2</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3593,7 +3593,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -4492,18 +4492,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100B1DC67C611DD5E4D81775F9F3E26A7B2" ma:contentTypeVersion="16" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7f379a5812b480a74f9d031be5f88a83">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xmlns:ns3="12535b08-222e-45d2-b6db-15019f1afee6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbce1e37d7de67e1c835013ca0ee7a7c" ns2:_="" ns3:_="">
     <xsd:import namespace="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
@@ -4744,6 +4732,18 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Zeit xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b63cdcf7-47fa-43f6-87e5-23b415b5c413">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="12535b08-222e-45d2-b6db-15019f1afee6" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{373398BC-AB18-4DB6-A1F8-8358A59BBA75}">
   <ds:schemaRefs>
@@ -4753,23 +4753,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84A691B-EF98-4CD8-ACB1-815521123DAC}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{981C8453-1A31-4F97-BF69-09535CFA9398}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4786,4 +4769,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B84A691B-EF98-4CD8-ACB1-815521123DAC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="12535b08-222e-45d2-b6db-15019f1afee6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b63cdcf7-47fa-43f6-87e5-23b415b5c413"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>